<commit_message>
add aligner option and extract unmapped reads options
</commit_message>
<xml_diff>
--- a/docs/UI/EDGE-v3-assembly-ui.xlsx
+++ b/docs/UI/EDGE-v3-assembly-ui.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lanl-my.sharepoint.com/personal/218819_win_lanl_gov/Documents/EDGEv3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andylo/Projects/LANL/EDGEv3/docs/UI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="188" documentId="8_{B718A015-77B2-FF4A-A3C2-82F5023228E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6781A11-9308-4845-9C29-5E325A065766}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0660AA64-AAC6-9742-B8F7-8C560565230F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26540" yWindow="-1720" windowWidth="30240" windowHeight="18880" xr2:uid="{079D525B-60B2-4B4A-BCF4-861050BE33CD}"/>
+    <workbookView xWindow="-30240" yWindow="-1720" windowWidth="30240" windowHeight="18880" xr2:uid="{079D525B-60B2-4B4A-BCF4-861050BE33CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="91">
   <si>
     <t>input</t>
   </si>
@@ -360,6 +360,77 @@
   </si>
   <si>
     <t>Reads Error-correction by racon using all-vs-all pairwise overlaps between reads including dual overlaps. This step is computationally intensive in terms of memory and time usage.</t>
+  </si>
+  <si>
+    <t>String? r2c_aligner_options</t>
+  </si>
+  <si>
+    <t>Boolean extractUnmapped</t>
+  </si>
+  <si>
+    <t>Aligner Options</t>
+  </si>
+  <si>
+    <t>Extract Unmapped/Unassembled Reads</t>
+  </si>
+  <si>
+    <r>
+      <t>Click </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bowtie2 (https://bowtie-bio.sourceforge.net/bowtie2/manual.shtml#usage)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF666666"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> | </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>BWA mem(https://bio-bwa.sourceforge.net/bwa.shtml#3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF666666"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> | </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Minimap2(https://lh3.github.io/minimap2/minimap2.html)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF666666"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> for detail. </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -407,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -416,7 +487,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,16 +821,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E938EBF4-18CD-3F42-BCDF-75AF1EF34683}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="5" max="5" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" customWidth="1"/>
     <col min="6" max="6" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -884,7 +954,7 @@
       <c r="F8" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1200,6 +1270,34 @@
       </c>
       <c r="F24" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>